<commit_message>
Se ajusta script de carga e insert
</commit_message>
<xml_diff>
--- a/Extraccion/outputs/Registro_Beneficiarios_Estrategias.xlsx
+++ b/Extraccion/outputs/Registro_Beneficiarios_Estrategias.xlsx
@@ -517,13 +517,25 @@
           <t>IE ARTURO GÓMEZ JARAMILLO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
@@ -548,13 +560,25 @@
           <t>IE SAN JOSÉ</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
@@ -579,13 +603,25 @@
           <t>IE EL PLACER</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
@@ -610,11 +646,19 @@
           <t>IE JORGE ISAACS</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -641,11 +685,19 @@
           <t>IE SANTA ANA DE LOS CABALLEROS</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -672,11 +724,19 @@
           <t>IE SANTA INÉS</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -704,10 +764,16 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
@@ -734,11 +800,19 @@
           <t>IE SANTA MARTA</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -765,11 +839,19 @@
           <t>IE EL ÁGUILA</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -796,11 +878,19 @@
           <t>IE JUSTINIANO ECHAVARRÍA</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -827,11 +917,19 @@
           <t>IE GILBERTO ÁLZATE AVENDAÑO</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
@@ -858,11 +956,19 @@
           <t>IE LA PRESENTACIÓN</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -890,10 +996,16 @@
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -921,10 +1033,16 @@
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
@@ -951,11 +1069,19 @@
           <t>IE SAN JOSÉ</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -983,10 +1109,16 @@
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1014,10 +1146,16 @@
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
@@ -1045,10 +1183,16 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1076,10 +1220,16 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1107,10 +1257,16 @@
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1137,11 +1293,19 @@
           <t>IE FRAY JOSÉ JOAQUÍN ESCOBAR</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1168,11 +1332,19 @@
           <t>IE TÉCNICA AGROPECUARIA TORO</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -1199,11 +1371,19 @@
           <t>IE NUESTRA SEÑORA DE LA CONSOLACIÓN</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1231,10 +1411,16 @@
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
@@ -1262,10 +1448,16 @@
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>

</xml_diff>